<commit_message>
Stetson Load Fix Color
</commit_message>
<xml_diff>
--- a/Excel/Stetson/2022.02.08/25.02.2022 STETSON — загрузка.xlsx
+++ b/Excel/Stetson/2022.02.08/25.02.2022 STETSON — загрузка.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F449576E-64EE-4E11-B5BD-6C6493B26862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADCDCCE4-6024-45EF-B907-E2CE9424D238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6DB72AB-BE88-4F7B-87DE-F28F56C0E962}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D73BB07E-9F1B-4047-A9D4-95B874D44610}"/>
   </bookViews>
   <sheets>
     <sheet name="Загрузка" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <author>general</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{2472006A-09B1-49F4-A621-19E15D75065D}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{9C95A200-E00E-42A2-B4B9-B493FB1A063B}">
       <text>
         <r>
           <rPr>
@@ -1375,8 +1375,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1385,12 +1383,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <b/>
@@ -1413,6 +1405,12 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1494,25 +1492,25 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 8" xfId="1" xr:uid="{9C01D06D-DBB6-4605-B753-030A728A4CAF}"/>
-    <cellStyle name="Финансовый 3" xfId="2" xr:uid="{D0F56C11-843B-4426-AC9A-30E083471591}"/>
+    <cellStyle name="Обычный 8" xfId="1" xr:uid="{8BB29441-3136-426D-B2EB-D96EC234CF58}"/>
+    <cellStyle name="Финансовый 3" xfId="2" xr:uid="{E17EFD7A-19D9-4B7D-885B-5827A49ADE5F}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1829,15 +1827,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E6CC40-2D13-4FA8-B6F3-8723394605F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A30F09-8866-40C2-94E8-60747B484370}">
   <sheetPr codeName="Лист28">
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:V128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AM121" sqref="AM121:AM127"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T122" sqref="T122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6485,7 +6483,7 @@
         <v>251</v>
       </c>
       <c r="U68" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V68" t="s">
         <v>252</v>
@@ -6621,7 +6619,7 @@
         <v>262</v>
       </c>
       <c r="U70" t="s">
-        <v>238</v>
+        <v>68</v>
       </c>
       <c r="V70" t="s">
         <v>263</v>
@@ -10087,7 +10085,7 @@
         <v>418</v>
       </c>
       <c r="U121" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V121" t="s">
         <v>419</v>
@@ -10155,7 +10153,7 @@
         <v>418</v>
       </c>
       <c r="U122" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V122" t="s">
         <v>419</v>
@@ -10223,7 +10221,7 @@
         <v>423</v>
       </c>
       <c r="U123" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V123" t="s">
         <v>424</v>
@@ -10291,7 +10289,7 @@
         <v>423</v>
       </c>
       <c r="U124" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V124" t="s">
         <v>424</v>
@@ -10359,7 +10357,7 @@
         <v>428</v>
       </c>
       <c r="U125" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V125" t="s">
         <v>429</v>
@@ -10427,7 +10425,7 @@
         <v>428</v>
       </c>
       <c r="U126" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V126" t="s">
         <v>429</v>
@@ -10495,7 +10493,7 @@
         <v>428</v>
       </c>
       <c r="U127" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="V127" t="s">
         <v>429</v>
@@ -10563,7 +10561,7 @@
         <v>433</v>
       </c>
       <c r="U128" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="V128" t="s">
         <v>434</v>
@@ -10576,7 +10574,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="U1:U1048576" xr:uid="{E32E3E76-ABFC-40B2-BB68-F3DF4C4A24F8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="U1:U1048576" xr:uid="{E61098B4-08A3-422C-94F7-1C4CE354523E}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>